<commit_message>
Update sheet for 2025-05-28
</commit_message>
<xml_diff>
--- a/CC Inspection Indy.xlsx
+++ b/CC Inspection Indy.xlsx
@@ -486,11 +486,7 @@
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
+      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">

</xml_diff>